<commit_message>
Update Order of an integer a mod n.xlsx
</commit_message>
<xml_diff>
--- a/Order of an integer a mod n.xlsx
+++ b/Order of an integer a mod n.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DougsDocuments\GitHub\Modulo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA1A169C-092C-49D7-8904-1ACF7138A2C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E666EB-534F-4BF0-8BDE-BD5C01F50E45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D4442487-E0D2-43F9-8513-211D30420B72}"/>
   </bookViews>
@@ -37,9 +37,6 @@
     <t>a</t>
   </si>
   <si>
-    <t>n =</t>
-  </si>
-  <si>
     <t>power of a →</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>inc =</t>
+  </si>
+  <si>
+    <t>mod n =</t>
   </si>
 </sst>
 </file>
@@ -78,18 +78,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -110,9 +104,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -122,11 +113,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -134,6 +128,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -458,27 +462,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="3.7109375" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B1" s="5">
-        <v>1</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="6"/>
+        <v>3</v>
+      </c>
+      <c r="B1" s="4">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="5"/>
     </row>
     <row r="2" spans="1:59" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="3">
+        <v>4</v>
+      </c>
+      <c r="B2" s="6">
         <v>13</v>
       </c>
       <c r="C2" s="1">
@@ -654,7 +658,7 @@
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1">
@@ -890,8 +894,8 @@
       </c>
     </row>
     <row r="4" spans="1:59" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3</v>
+      <c r="A4" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="B4" s="1">
         <f t="shared" ref="B4:B35" si="3">B3+$B$1</f>
@@ -22191,8 +22195,11 @@
     <mergeCell ref="C1:D1"/>
   </mergeCells>
   <conditionalFormatting sqref="C3:BG94">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
       <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>